<commit_message>
Updat 14th Of May 2023
</commit_message>
<xml_diff>
--- a/IPL/Data/exp/pstats_tpose_v01_Gujarat Titans.xlsx
+++ b/IPL/Data/exp/pstats_tpose_v01_Gujarat Titans.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1364,32 +1364,32 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>balls_faced_pp</t>
+          <t>runs_mid</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="D14" t="n">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="E14" t="n">
+        <v>97</v>
+      </c>
+      <c r="F14" t="n">
+        <v>112</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>1</v>
       </c>
-      <c r="F14" t="n">
-        <v>10</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -1419,32 +1419,32 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>outs_pp</t>
+          <t>runs_dth</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -1474,32 +1474,32 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>runs_mid</t>
+          <t>outs_pp</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -1529,32 +1529,32 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>balls_faced_mid</t>
+          <t>outs_mid</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>112</v>
+        <v>5</v>
       </c>
       <c r="E17" t="n">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -1584,33 +1584,33 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>outs_mid</t>
+          <t>outs_dth</t>
         </is>
       </c>
       <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
         <v>1</v>
       </c>
-      <c r="C18" t="n">
-        <v>5</v>
-      </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" t="n">
         <v>1</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
         <v>3</v>
       </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>2</v>
-      </c>
       <c r="J18" t="n">
         <v>0</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -1639,32 +1639,32 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>runs_dth</t>
+          <t>tout_pace</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D19" t="n">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="G19" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
@@ -1694,32 +1694,32 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>balls_faced_dth</t>
+          <t>tout_spin</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E20" t="n">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
@@ -1749,32 +1749,32 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>outs_dth</t>
+          <t>balls_faced_pp</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="C21" t="n">
+        <v>115</v>
+      </c>
+      <c r="D21" t="n">
+        <v>48</v>
+      </c>
+      <c r="E21" t="n">
         <v>1</v>
       </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="n">
-        <v>3</v>
-      </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1792,7 +1792,7 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
@@ -1804,32 +1804,32 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>fantasy_pts_30</t>
+          <t>balls_faced_mid</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C22" t="n">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="E22" t="n">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="F22" t="n">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I22" t="n">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1847,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
@@ -1859,32 +1859,32 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>fantasy_pts_50</t>
+          <t>balls_faced_dth</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="F23" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
@@ -1914,23 +1914,23 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>fantasy_pts_100</t>
+          <t>fantasy_pts_30</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P24" t="n">
         <v>0</v>
@@ -1969,23 +1969,23 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>fantasy_pts_0</t>
+          <t>fantasy_pts_50</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>-2</v>
+        <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E25" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
@@ -2024,7 +2024,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>t_balls_bowled</t>
+          <t>fantasy_pts_100</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -2043,98 +2043,98 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>216</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="O26" t="n">
         <v>0</v>
       </c>
       <c r="P26" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>t_runs_conceded</t>
+          <t>fantasy_pts_0</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D27" t="n">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>306</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>233</v>
+        <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
       <c r="O27" t="n">
         <v>0</v>
       </c>
       <c r="P27" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>overs_bowled_pp</t>
+          <t>t_balls_bowled</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -2153,43 +2153,43 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="K28" t="n">
-        <v>25</v>
+        <v>210</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="M28" t="n">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="N28" t="n">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
       </c>
       <c r="P28" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="Q28" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>overs_bowled_mid</t>
+          <t>t_runs_conceded</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -2199,52 +2199,52 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
+        <v>129</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>306</v>
+      </c>
+      <c r="H29" t="n">
         <v>7</v>
       </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>25</v>
-      </c>
-      <c r="H29" t="n">
-        <v>1</v>
-      </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="K29" t="n">
-        <v>2</v>
+        <v>233</v>
       </c>
       <c r="L29" t="n">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="M29" t="n">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="N29" t="n">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="O29" t="n">
         <v>0</v>
       </c>
       <c r="P29" t="n">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="Q29" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>overs_bowled_dth</t>
+          <t>wkts_pp</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -2263,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -2272,25 +2272,25 @@
         <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
         <v>2</v>
       </c>
-      <c r="N30" t="n">
-        <v>7</v>
-      </c>
       <c r="O30" t="n">
         <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -2299,7 +2299,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>runs_conceded_pp</t>
+          <t>wkts_mid</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -2327,19 +2327,19 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K31" t="n">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M31" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="N31" t="n">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="O31" t="n">
         <v>0</v>
@@ -2348,13 +2348,13 @@
         <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>runs_conceded_mid</t>
+          <t>wkts_dth</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -2364,7 +2364,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -2373,43 +2373,43 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>206</v>
+        <v>6</v>
       </c>
       <c r="H32" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="K32" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="L32" t="n">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="M32" t="n">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="N32" t="n">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>runs_conceded_dth</t>
+          <t>overs_bowled_pp</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2437,34 +2437,34 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="L33" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="M33" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N33" t="n">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>wkts_pp</t>
+          <t>overs_bowled_mid</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -2483,43 +2483,43 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
+        <v>25</v>
+      </c>
+      <c r="H34" t="n">
         <v>1</v>
       </c>
-      <c r="H34" t="n">
-        <v>0</v>
-      </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K34" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N34" t="n">
+        <v>8</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q34" t="n">
         <v>2</v>
-      </c>
-      <c r="O34" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>wkts_mid</t>
+          <t>overs_bowled_dth</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -2538,34 +2538,34 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
+        <v>7</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>7</v>
+      </c>
+      <c r="K35" t="n">
         <v>8</v>
       </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
+      <c r="L35" t="n">
+        <v>4</v>
+      </c>
+      <c r="M35" t="n">
         <v>2</v>
       </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>6</v>
-      </c>
-      <c r="M35" t="n">
-        <v>4</v>
-      </c>
       <c r="N35" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O35" t="n">
         <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q35" t="n">
         <v>0</v>
@@ -2574,7 +2574,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>wkts_dth</t>
+          <t>runs_conceded_pp</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -2602,19 +2602,19 @@
         <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K36" t="n">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="L36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="N36" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2623,160 +2623,174 @@
         <v>0</v>
       </c>
       <c r="Q36" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>batting_team</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr"/>
-      <c r="K37" t="inlineStr"/>
-      <c r="L37" t="inlineStr"/>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
+          <t>runs_conceded_mid</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>52</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>206</v>
+      </c>
+      <c r="H37" t="n">
+        <v>7</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>75</v>
+      </c>
+      <c r="K37" t="n">
+        <v>14</v>
+      </c>
+      <c r="L37" t="n">
+        <v>97</v>
+      </c>
+      <c r="M37" t="n">
+        <v>133</v>
+      </c>
+      <c r="N37" t="n">
+        <v>62</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>64</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>batsman</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>WP Saha</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Shubman Gill</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>HH Pandya</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>DA Miller</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>V Shankar</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>Rashid Khan</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>R Tewatia</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>A Manohar</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr"/>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>B Sai Sudharsan</t>
-        </is>
-      </c>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
+          <t>runs_conceded_dth</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>62</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>43</v>
+      </c>
+      <c r="K38" t="n">
+        <v>80</v>
+      </c>
+      <c r="L38" t="n">
+        <v>24</v>
+      </c>
+      <c r="M38" t="n">
+        <v>14</v>
+      </c>
+      <c r="N38" t="n">
+        <v>75</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>runs_in_1st_over</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>25</v>
-      </c>
-      <c r="C39" t="n">
-        <v>63</v>
-      </c>
-      <c r="D39" t="n">
-        <v>8</v>
-      </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="n">
-        <v>27</v>
-      </c>
-      <c r="G39" t="n">
-        <v>10</v>
-      </c>
-      <c r="H39" t="n">
-        <v>15</v>
-      </c>
-      <c r="I39" t="inlineStr"/>
+          <t>batting_team</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
-      <c r="O39" t="n">
-        <v>22</v>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
       </c>
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
@@ -2784,34 +2798,58 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>runs_in_7th_over</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>14</v>
-      </c>
-      <c r="C40" t="n">
-        <v>14</v>
-      </c>
-      <c r="D40" t="n">
-        <v>5</v>
-      </c>
-      <c r="E40" t="n">
-        <v>31</v>
-      </c>
-      <c r="F40" t="n">
-        <v>29</v>
-      </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
+          <t>batsman</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>WP Saha</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Shubman Gill</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>HH Pandya</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>DA Miller</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>V Shankar</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Rashid Khan</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>R Tewatia</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>A Manohar</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
-      <c r="O40" t="n">
-        <v>62</v>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>B Sai Sudharsan</t>
+        </is>
       </c>
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
@@ -2819,34 +2857,36 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>runs_in_13th_over</t>
+          <t>tr.G01</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C41" t="n">
-        <v>39</v>
-      </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="n">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D41" t="n">
+        <v>8</v>
+      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>63</v>
-      </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="n">
-        <v>14</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G41" t="n">
+        <v>10</v>
+      </c>
+      <c r="H41" t="n">
+        <v>15</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="n">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
@@ -2854,26 +2894,26 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>runs_in_18th_over</t>
+          <t>tr.G07</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C42" t="n">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="D42" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E42" t="n">
-        <v>17</v>
-      </c>
-      <c r="F42" t="inlineStr"/>
+        <v>31</v>
+      </c>
+      <c r="F42" t="n">
+        <v>29</v>
+      </c>
       <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
-        <v>5</v>
-      </c>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
@@ -2881,7 +2921,7 @@
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="n">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
@@ -2889,30 +2929,26 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>runs_in_23rd_over</t>
+          <t>tr.G13</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C43" t="n">
-        <v>45</v>
-      </c>
-      <c r="D43" t="n">
-        <v>28</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>46</v>
-      </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F43" t="n">
+        <v>63</v>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
       <c r="I43" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
@@ -2920,7 +2956,7 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="n">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
@@ -2928,103 +2964,105 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>runs_in_30th_over</t>
+          <t>tr.G18</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="D44" t="n">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="E44" t="n">
-        <v>6</v>
-      </c>
-      <c r="F44" t="n">
-        <v>10</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
-        <v>2</v>
-      </c>
-      <c r="I44" t="n">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
+      <c r="O44" t="n">
+        <v>19</v>
+      </c>
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>runs_in_35th_over</t>
+          <t>tr.G23</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D45" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E45" t="n">
         <v>46</v>
       </c>
-      <c r="F45" t="n">
-        <v>19</v>
-      </c>
+      <c r="F45" t="inlineStr"/>
       <c r="G45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
-      <c r="O45" t="inlineStr"/>
+      <c r="O45" t="n">
+        <v>20</v>
+      </c>
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>runs_in_39th_over</t>
+          <t>tr.G30</t>
         </is>
       </c>
       <c r="B46" t="n">
+        <v>47</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>66</v>
+      </c>
+      <c r="E46" t="n">
+        <v>6</v>
+      </c>
+      <c r="F46" t="n">
         <v>10</v>
       </c>
-      <c r="C46" t="n">
-        <v>49</v>
-      </c>
-      <c r="D46" t="n">
-        <v>26</v>
-      </c>
-      <c r="E46" t="n">
-        <v>32</v>
-      </c>
-      <c r="F46" t="n">
-        <v>51</v>
-      </c>
       <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
+      <c r="H46" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" t="n">
+        <v>3</v>
+      </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="inlineStr"/>
@@ -3037,32 +3075,32 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>runs_in_44th_over</t>
+          <t>tr.G35</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="D47" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F47" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G47" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H47" t="n">
         <v>20</v>
       </c>
       <c r="I47" t="n">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
@@ -3076,218 +3114,222 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>bowling_team</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
+          <t>tr.G39</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>10</v>
+      </c>
+      <c r="C48" t="n">
+        <v>49</v>
+      </c>
+      <c r="D48" t="n">
+        <v>26</v>
+      </c>
+      <c r="E48" t="n">
+        <v>32</v>
+      </c>
+      <c r="F48" t="n">
+        <v>51</v>
+      </c>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>Gujarat Titans</t>
-        </is>
-      </c>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>bowler</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>HH Pandya</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Rashid Khan</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>R Tewatia</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>MM Sharma</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Mohammed Shami</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>Noor Ahmad</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>AS Joseph</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>J Little</t>
-        </is>
-      </c>
+          <t>tr.G44</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>6</v>
+      </c>
+      <c r="D49" t="n">
+        <v>59</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>6</v>
+      </c>
+      <c r="G49" t="n">
+        <v>3</v>
+      </c>
+      <c r="H49" t="n">
+        <v>20</v>
+      </c>
+      <c r="I49" t="n">
+        <v>26</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Yash Dayal</t>
-        </is>
-      </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>J Yadav</t>
-        </is>
-      </c>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_1st_over</t>
+          <t>bowling_team</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="n">
-        <v>0</v>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr"/>
-      <c r="G50" t="n">
-        <v>2</v>
-      </c>
-      <c r="H50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
       <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="n">
-        <v>2</v>
-      </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="n">
-        <v>2</v>
-      </c>
-      <c r="N50" t="n">
-        <v>1</v>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
       </c>
       <c r="O50" t="inlineStr"/>
-      <c r="P50" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q50" t="inlineStr"/>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>Gujarat Titans</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_7th_over</t>
+          <t>bowler</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
-        <v>0</v>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>HH Pandya</t>
+        </is>
       </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr"/>
-      <c r="G51" t="n">
-        <v>3</v>
-      </c>
-      <c r="H51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Rashid Khan</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>R Tewatia</t>
+        </is>
+      </c>
       <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="n">
-        <v>3</v>
-      </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="n">
-        <v>2</v>
-      </c>
-      <c r="N51" t="n">
-        <v>0</v>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>MM Sharma</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Mohammed Shami</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Noor Ahmad</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>AS Joseph</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>J Little</t>
+        </is>
       </c>
       <c r="O51" t="inlineStr"/>
-      <c r="P51" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q51" t="inlineStr"/>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Yash Dayal</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>J Yadav</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_13th_over</t>
+          <t>tbwkt.G01</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr"/>
       <c r="G52" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="n">
@@ -3305,112 +3347,108 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_18th_over</t>
+          <t>tbwkt.G07</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr"/>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
-      <c r="J53" t="n">
-        <v>2</v>
-      </c>
+      <c r="J53" t="inlineStr"/>
       <c r="K53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N53" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
       <c r="Q53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_23rd_over</t>
+          <t>tbwkt.G13</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
-        <v>1</v>
-      </c>
+      <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr"/>
       <c r="G54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
-      <c r="J54" t="n">
-        <v>0</v>
-      </c>
+      <c r="J54" t="inlineStr"/>
       <c r="K54" t="n">
-        <v>3</v>
-      </c>
-      <c r="L54" t="n">
         <v>1</v>
       </c>
+      <c r="L54" t="inlineStr"/>
       <c r="M54" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="N54" t="n">
+        <v>1</v>
+      </c>
       <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
       <c r="Q54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_30th_over</t>
+          <t>tbwkt.G18</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
-      <c r="D55" t="n">
-        <v>0</v>
-      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr"/>
       <c r="G55" t="n">
         <v>1</v>
       </c>
-      <c r="H55" t="n">
-        <v>0</v>
-      </c>
+      <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" t="n">
-        <v>2</v>
-      </c>
-      <c r="M55" t="inlineStr"/>
-      <c r="N55" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="n">
+        <v>1</v>
+      </c>
+      <c r="N55" t="n">
+        <v>3</v>
+      </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_35th_over</t>
+          <t>tbwkt.G23</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -3426,18 +3464,18 @@
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
         <v>3</v>
       </c>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
       <c r="L56" t="n">
-        <v>3</v>
-      </c>
-      <c r="M56" t="inlineStr"/>
-      <c r="N56" t="n">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
@@ -3445,7 +3483,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_39th_over</t>
+          <t>tbwkt.G30</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -3456,31 +3494,33 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr"/>
       <c r="G57" t="n">
-        <v>0</v>
-      </c>
-      <c r="H57" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K57" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L57" t="n">
         <v>2</v>
       </c>
       <c r="M57" t="inlineStr"/>
-      <c r="N57" t="n">
-        <v>2</v>
-      </c>
+      <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
+      <c r="Q57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>wkts_in_44th_over</t>
+          <t>tbwkt.G35</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -3491,18 +3531,18 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr"/>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K58" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M58" t="inlineStr"/>
       <c r="N58" t="n">
@@ -3515,114 +3555,102 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>run_rate_pp</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>91</v>
-      </c>
-      <c r="C59" t="n">
-        <v>49</v>
-      </c>
+          <t>tbwkt.G39</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
       <c r="D59" t="n">
-        <v>23</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
         <v>3</v>
       </c>
-      <c r="G59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" t="inlineStr"/>
-      <c r="K59" t="inlineStr"/>
-      <c r="L59" t="inlineStr"/>
+      <c r="L59" t="n">
+        <v>2</v>
+      </c>
       <c r="M59" t="inlineStr"/>
-      <c r="N59" t="inlineStr"/>
-      <c r="O59" t="n">
-        <v>34</v>
-      </c>
+      <c r="N59" t="n">
+        <v>2</v>
+      </c>
+      <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>run_rate_mid</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>9</v>
-      </c>
-      <c r="C60" t="n">
-        <v>47</v>
-      </c>
+          <t>tbwkt.G44</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
-        <v>59</v>
-      </c>
-      <c r="E60" t="n">
-        <v>54</v>
-      </c>
-      <c r="F60" t="n">
-        <v>55</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
       <c r="G60" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="n">
         <v>2</v>
       </c>
-      <c r="I60" t="n">
-        <v>57</v>
-      </c>
-      <c r="J60" t="inlineStr"/>
-      <c r="K60" t="inlineStr"/>
-      <c r="L60" t="inlineStr"/>
+      <c r="K60" t="n">
+        <v>4</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
       <c r="M60" t="inlineStr"/>
-      <c r="N60" t="inlineStr"/>
-      <c r="O60" t="n">
-        <v>55</v>
-      </c>
+      <c r="N60" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>run_rate_dth</t>
+          <t>runmix_%_pp</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D61" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E61" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="G61" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
@@ -3630,7 +3658,7 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
@@ -3638,274 +3666,236 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>t_runs</t>
+          <t>runmix_%_mid</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="C62" t="n">
-        <v>339</v>
+        <v>47</v>
       </c>
       <c r="D62" t="n">
-        <v>213</v>
+        <v>59</v>
       </c>
       <c r="E62" t="n">
-        <v>180</v>
+        <v>54</v>
       </c>
       <c r="F62" t="n">
-        <v>205</v>
+        <v>55</v>
       </c>
       <c r="G62" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="H62" t="n">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="I62" t="n">
-        <v>112</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0</v>
-      </c>
-      <c r="L62" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" t="n">
-        <v>0</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
       <c r="O62" t="n">
-        <v>176</v>
-      </c>
-      <c r="P62" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q62" t="n">
-        <v>0</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>t_innings</t>
+          <t>runmix_%_dth</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D63" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E63" t="n">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F63" t="n">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="G63" t="n">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="H63" t="n">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="I63" t="n">
-        <v>5</v>
-      </c>
-      <c r="J63" t="n">
-        <v>6</v>
-      </c>
-      <c r="K63" t="n">
-        <v>9</v>
-      </c>
-      <c r="L63" t="n">
-        <v>5</v>
-      </c>
-      <c r="M63" t="n">
-        <v>5</v>
-      </c>
-      <c r="N63" t="n">
-        <v>7</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
       <c r="O63" t="n">
-        <v>5</v>
-      </c>
-      <c r="P63" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q63" t="n">
-        <v>1</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>overs_bowled_rate_pp</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr"/>
-      <c r="C64" t="inlineStr"/>
+          <t>tr%.pace</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>77</v>
+      </c>
+      <c r="C64" t="n">
+        <v>52</v>
+      </c>
       <c r="D64" t="n">
-        <v>59</v>
-      </c>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
+        <v>48</v>
+      </c>
+      <c r="E64" t="n">
+        <v>49</v>
+      </c>
+      <c r="F64" t="n">
+        <v>54</v>
+      </c>
       <c r="G64" t="n">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="H64" t="n">
-        <v>0</v>
-      </c>
-      <c r="I64" t="inlineStr"/>
-      <c r="J64" t="n">
-        <v>6</v>
-      </c>
-      <c r="K64" t="n">
-        <v>71</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" t="n">
-        <v>11</v>
-      </c>
-      <c r="N64" t="n">
-        <v>40</v>
-      </c>
-      <c r="O64" t="inlineStr"/>
-      <c r="P64" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q64" t="n">
-        <v>50</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I64" t="n">
+        <v>54</v>
+      </c>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="n">
+        <v>57</v>
+      </c>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>overs_bowled_rate_mid</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
+          <t>tr%.spin</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>23</v>
+      </c>
+      <c r="C65" t="n">
+        <v>48</v>
+      </c>
       <c r="D65" t="n">
-        <v>41</v>
-      </c>
-      <c r="E65" t="inlineStr"/>
-      <c r="F65" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="E65" t="n">
+        <v>51</v>
+      </c>
+      <c r="F65" t="n">
+        <v>46</v>
+      </c>
       <c r="G65" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>100</v>
-      </c>
-      <c r="I65" t="inlineStr"/>
-      <c r="J65" t="n">
-        <v>56</v>
-      </c>
-      <c r="K65" t="n">
-        <v>6</v>
-      </c>
-      <c r="L65" t="n">
-        <v>79</v>
-      </c>
-      <c r="M65" t="n">
-        <v>79</v>
-      </c>
-      <c r="N65" t="n">
-        <v>32</v>
-      </c>
-      <c r="O65" t="inlineStr"/>
-      <c r="P65" t="n">
-        <v>83</v>
-      </c>
-      <c r="Q65" t="n">
-        <v>50</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I65" t="n">
+        <v>46</v>
+      </c>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="n">
+        <v>43</v>
+      </c>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>overs_bowled_rate_dth</t>
+          <t>wicketmix_%_rate_pp</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
-        <v>19</v>
-      </c>
-      <c r="H66" t="n">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="K66" t="n">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="L66" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="M66" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="N66" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O66" t="inlineStr"/>
-      <c r="P66" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q66" t="n">
-        <v>0</v>
-      </c>
+      <c r="P66" t="inlineStr"/>
+      <c r="Q66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>wicketotal_rate_pp</t>
+          <t>wicketmix_%_rate_mid</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K67" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="L67" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="M67" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="N67" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="inlineStr"/>
@@ -3914,7 +3904,7 @@
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>wicketotal_rate_mid</t>
+          <t>wicketmix_%_rate_dth</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -3925,24 +3915,24 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr"/>
       <c r="G68" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="n">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="K68" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="L68" t="n">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="M68" t="n">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="N68" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
@@ -3951,35 +3941,35 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>wicketotal_rate_dth</t>
+          <t>tbwkt%.lhb</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr"/>
       <c r="G69" t="n">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="n">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="K69" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L69" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="M69" t="n">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="N69" t="n">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr"/>
@@ -3988,208 +3978,955 @@
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>total_wickets</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>0</v>
-      </c>
-      <c r="C70" t="n">
-        <v>0</v>
-      </c>
+          <t>tbwkt%.rhb</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
       <c r="D70" t="n">
-        <v>3</v>
-      </c>
-      <c r="E70" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" t="n">
-        <v>15</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I70" t="n">
-        <v>0</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
       <c r="J70" t="n">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="K70" t="n">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="L70" t="n">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="M70" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="N70" t="n">
-        <v>7</v>
-      </c>
-      <c r="O70" t="n">
-        <v>0</v>
-      </c>
-      <c r="P70" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q70" t="n">
-        <v>0</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>total_overs_bowled</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>0</v>
-      </c>
-      <c r="C71" t="n">
-        <v>0</v>
-      </c>
+          <t>overmix_%_pp</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
       <c r="D71" t="n">
-        <v>17</v>
-      </c>
-      <c r="E71" t="n">
-        <v>0</v>
-      </c>
-      <c r="F71" t="n">
-        <v>0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
       <c r="G71" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="H71" t="n">
-        <v>1</v>
-      </c>
-      <c r="I71" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr"/>
       <c r="J71" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K71" t="n">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="L71" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="M71" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="N71" t="n">
-        <v>25</v>
-      </c>
-      <c r="O71" t="n">
-        <v>0</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="O71" t="inlineStr"/>
       <c r="P71" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q71" t="n">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>runs_innings_ratio</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>17</v>
-      </c>
-      <c r="C72" t="n">
-        <v>38</v>
-      </c>
+          <t>overmix_%_rate_mid</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
       <c r="D72" t="n">
-        <v>27</v>
-      </c>
-      <c r="E72" t="n">
-        <v>22</v>
-      </c>
-      <c r="F72" t="n">
-        <v>29</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
       <c r="G72" t="n">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="H72" t="n">
-        <v>10</v>
-      </c>
-      <c r="I72" t="n">
-        <v>22</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="I72" t="inlineStr"/>
       <c r="J72" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="K72" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L72" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="M72" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="N72" t="n">
-        <v>0</v>
-      </c>
-      <c r="O72" t="n">
-        <v>35</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="O72" t="inlineStr"/>
       <c r="P72" t="n">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="Q72" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>4xtbwkt_tbov_ratio</t>
+          <t>overmix_%_rate_dth</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="n">
-        <v>1.7</v>
+        <v>19</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
       </c>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="n">
-        <v>2.4</v>
+        <v>39</v>
       </c>
       <c r="K73" t="n">
-        <v>1.9</v>
+        <v>23</v>
       </c>
       <c r="L73" t="n">
-        <v>1.7</v>
+        <v>21</v>
       </c>
       <c r="M73" t="n">
-        <v>1.5</v>
+        <v>11</v>
       </c>
       <c r="N73" t="n">
-        <v>1.1</v>
+        <v>28</v>
       </c>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="Q73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>tbov%.rhb</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>82</v>
+      </c>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="n">
+        <v>83</v>
+      </c>
+      <c r="H74" t="n">
+        <v>100</v>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="n">
+        <v>83</v>
+      </c>
+      <c r="K74" t="n">
+        <v>86</v>
+      </c>
+      <c r="L74" t="n">
+        <v>95</v>
+      </c>
+      <c r="M74" t="n">
+        <v>79</v>
+      </c>
+      <c r="N74" t="n">
+        <v>80</v>
+      </c>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>tbov%.lhb</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="n">
+        <v>82</v>
+      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="n">
+        <v>89</v>
+      </c>
+      <c r="H75" t="n">
+        <v>100</v>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="n">
+        <v>72</v>
+      </c>
+      <c r="K75" t="n">
+        <v>69</v>
+      </c>
+      <c r="L75" t="n">
+        <v>89</v>
+      </c>
+      <c r="M75" t="n">
+        <v>89</v>
+      </c>
+      <c r="N75" t="n">
+        <v>80</v>
+      </c>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="n">
+        <v>83</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>t_innings</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>9</v>
+      </c>
+      <c r="C76" t="n">
+        <v>9</v>
+      </c>
+      <c r="D76" t="n">
+        <v>8</v>
+      </c>
+      <c r="E76" t="n">
+        <v>8</v>
+      </c>
+      <c r="F76" t="n">
+        <v>7</v>
+      </c>
+      <c r="G76" t="n">
+        <v>9</v>
+      </c>
+      <c r="H76" t="n">
+        <v>6</v>
+      </c>
+      <c r="I76" t="n">
+        <v>5</v>
+      </c>
+      <c r="J76" t="n">
+        <v>6</v>
+      </c>
+      <c r="K76" t="n">
+        <v>9</v>
+      </c>
+      <c r="L76" t="n">
+        <v>5</v>
+      </c>
+      <c r="M76" t="n">
+        <v>5</v>
+      </c>
+      <c r="N76" t="n">
+        <v>7</v>
+      </c>
+      <c r="O76" t="n">
+        <v>5</v>
+      </c>
+      <c r="P76" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>t_runs</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>151</v>
+      </c>
+      <c r="C77" t="n">
+        <v>339</v>
+      </c>
+      <c r="D77" t="n">
+        <v>213</v>
+      </c>
+      <c r="E77" t="n">
+        <v>180</v>
+      </c>
+      <c r="F77" t="n">
+        <v>205</v>
+      </c>
+      <c r="G77" t="n">
+        <v>16</v>
+      </c>
+      <c r="H77" t="n">
+        <v>63</v>
+      </c>
+      <c r="I77" t="n">
+        <v>112</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="n">
+        <v>176</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>tr_pace</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>116</v>
+      </c>
+      <c r="C78" t="n">
+        <v>177</v>
+      </c>
+      <c r="D78" t="n">
+        <v>103</v>
+      </c>
+      <c r="E78" t="n">
+        <v>89</v>
+      </c>
+      <c r="F78" t="n">
+        <v>110</v>
+      </c>
+      <c r="G78" t="n">
+        <v>16</v>
+      </c>
+      <c r="H78" t="n">
+        <v>62</v>
+      </c>
+      <c r="I78" t="n">
+        <v>61</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="n">
+        <v>100</v>
+      </c>
+      <c r="P78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>tr_spin</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>35</v>
+      </c>
+      <c r="C79" t="n">
+        <v>162</v>
+      </c>
+      <c r="D79" t="n">
+        <v>110</v>
+      </c>
+      <c r="E79" t="n">
+        <v>91</v>
+      </c>
+      <c r="F79" t="n">
+        <v>95</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>1</v>
+      </c>
+      <c r="I79" t="n">
+        <v>51</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="n">
+        <v>76</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>tout</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>9</v>
+      </c>
+      <c r="C80" t="n">
+        <v>10</v>
+      </c>
+      <c r="D80" t="n">
+        <v>7</v>
+      </c>
+      <c r="E80" t="n">
+        <v>4</v>
+      </c>
+      <c r="F80" t="n">
+        <v>5</v>
+      </c>
+      <c r="G80" t="n">
+        <v>1</v>
+      </c>
+      <c r="H80" t="n">
+        <v>1</v>
+      </c>
+      <c r="I80" t="n">
+        <v>5</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="n">
+        <v>3</v>
+      </c>
+      <c r="P80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>total_overs_bowled</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>0</v>
+      </c>
+      <c r="D81" t="n">
+        <v>17</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>36</v>
+      </c>
+      <c r="H81" t="n">
+        <v>1</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="n">
+        <v>18</v>
+      </c>
+      <c r="K81" t="n">
+        <v>35</v>
+      </c>
+      <c r="L81" t="n">
+        <v>19</v>
+      </c>
+      <c r="M81" t="n">
+        <v>19</v>
+      </c>
+      <c r="N81" t="n">
+        <v>25</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>tbov_rhb</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" t="n">
+        <v>0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>14</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>30</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="n">
+        <v>15</v>
+      </c>
+      <c r="K82" t="n">
+        <v>30</v>
+      </c>
+      <c r="L82" t="n">
+        <v>18</v>
+      </c>
+      <c r="M82" t="n">
+        <v>15</v>
+      </c>
+      <c r="N82" t="n">
+        <v>20</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>tbov_lhb</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>14</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>32</v>
+      </c>
+      <c r="H83" t="n">
+        <v>1</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" t="n">
+        <v>13</v>
+      </c>
+      <c r="K83" t="n">
+        <v>24</v>
+      </c>
+      <c r="L83" t="n">
+        <v>17</v>
+      </c>
+      <c r="M83" t="n">
+        <v>17</v>
+      </c>
+      <c r="N83" t="n">
+        <v>20</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>total_wickets</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>3</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>15</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="n">
+        <v>11</v>
+      </c>
+      <c r="K84" t="n">
+        <v>17</v>
+      </c>
+      <c r="L84" t="n">
+        <v>8</v>
+      </c>
+      <c r="M84" t="n">
+        <v>7</v>
+      </c>
+      <c r="N84" t="n">
+        <v>7</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>tbwkt_rhb</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>7</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="n">
+        <v>6</v>
+      </c>
+      <c r="K85" t="n">
+        <v>12</v>
+      </c>
+      <c r="L85" t="n">
+        <v>5</v>
+      </c>
+      <c r="M85" t="n">
+        <v>1</v>
+      </c>
+      <c r="N85" t="n">
+        <v>3</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>tbwkt_lhb</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>8</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="n">
+        <v>5</v>
+      </c>
+      <c r="K86" t="n">
+        <v>4</v>
+      </c>
+      <c r="L86" t="n">
+        <v>3</v>
+      </c>
+      <c r="M86" t="n">
+        <v>6</v>
+      </c>
+      <c r="N86" t="n">
+        <v>4</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>runs_innings_ratio</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>17</v>
+      </c>
+      <c r="C87" t="n">
+        <v>38</v>
+      </c>
+      <c r="D87" t="n">
+        <v>27</v>
+      </c>
+      <c r="E87" t="n">
+        <v>22</v>
+      </c>
+      <c r="F87" t="n">
+        <v>29</v>
+      </c>
+      <c r="G87" t="n">
+        <v>2</v>
+      </c>
+      <c r="H87" t="n">
+        <v>10</v>
+      </c>
+      <c r="I87" t="n">
+        <v>22</v>
+      </c>
+      <c r="J87" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="n">
+        <v>35</v>
+      </c>
+      <c r="P87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>4xtbwkt_tbov_ratio</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="K88" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="L88" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="M88" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="N88" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>